<commit_message>
Finally ran on both datasets without error
</commit_message>
<xml_diff>
--- a/DD_Project/data/Knudsen/statistical_tests/statistical_tests_results.xlsx
+++ b/DD_Project/data/Knudsen/statistical_tests/statistical_tests_results.xlsx
@@ -517,12 +517,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>0.762059105914683</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.303614051408536</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7255255521465513</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.3520814310313832</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.388936515176701e-09</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-5.968875949046395</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
@@ -532,12 +544,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>5.686511040792311e-09</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-6.381047079731257</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5.351620493450325e-09</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-6.39416387862277</v>
+      </c>
+      <c r="H3" t="n">
+        <v>9.016129832542732e-109</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-22.15657048241658</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
@@ -547,12 +571,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>3.422543139328303e-13</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8.393353377635671</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.784682725895748e-13</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8.434835395888939</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3.458822591901811e-30</v>
+      </c>
+      <c r="I4" t="n">
+        <v>11.41650059352173</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
@@ -562,12 +598,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>5.355966580390329e-15</v>
+      </c>
+      <c r="E5" t="n">
+        <v>9.225269478420378</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.341430691584698e-15</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9.319294238537607</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.982370483193783e-32</v>
+      </c>
+      <c r="I5" t="n">
+        <v>11.85687476417566</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -577,12 +625,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>1.323525533984203e-19</v>
+      </c>
+      <c r="E6" t="n">
+        <v>11.34293864385053</v>
+      </c>
+      <c r="F6" t="n">
+        <v>7.845346632130194e-20</v>
+      </c>
+      <c r="G6" t="n">
+        <v>11.44824383256682</v>
+      </c>
+      <c r="H6" t="n">
+        <v>7.934603239132094e-77</v>
+      </c>
+      <c r="I6" t="n">
+        <v>18.55147397768945</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
@@ -596,12 +656,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>0.8055216933659259</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.2468678510748198</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8208481120629288</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.2270563775176545</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6.913298295964885e-05</v>
+      </c>
+      <c r="I7" t="n">
+        <v>3.979250108044303</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
@@ -611,12 +683,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>5.496864632841192e-27</v>
+      </c>
+      <c r="E8" t="n">
+        <v>14.87623964976418</v>
+      </c>
+      <c r="F8" t="n">
+        <v>5.129544810442881e-27</v>
+      </c>
+      <c r="G8" t="n">
+        <v>14.89121838209819</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7.613453626347088e-148</v>
+      </c>
+      <c r="I8" t="n">
+        <v>25.89483948601856</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
@@ -626,12 +710,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>2.062060594623203e-30</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-16.62536113409849</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.436103272338343e-30</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-16.70768304585782</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.252407922159089e-205</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-30.5992497947913</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
@@ -641,12 +737,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>5.424127660214918e-22</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-12.45834829903501</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.268935992250986e-22</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-12.50742647079036</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4.202964353333529e-63</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-16.76772482371776</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
@@ -656,12 +764,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>4.625035176885589e-18</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-10.63068206484681</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3.60104621657e-18</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-10.68067968395436</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2.711897858146409e-67</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-17.3317005614847</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -675,12 +795,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>0.07999313799990201</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.768883195707782</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.08507137819118803</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.739406539211739</v>
+      </c>
+      <c r="H12" t="n">
+        <v>9.678239176902329e-07</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4.898070340087965</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
@@ -690,12 +822,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>1.764144515437736e-32</v>
+      </c>
+      <c r="E13" t="n">
+        <v>17.7249474552196</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.687595318396552e-32</v>
+      </c>
+      <c r="G13" t="n">
+        <v>17.73536196466344</v>
+      </c>
+      <c r="H13" t="n">
+        <v>8.951368322799402e-157</v>
+      </c>
+      <c r="I13" t="n">
+        <v>26.67594793592158</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
@@ -705,12 +849,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>9.494735343368508e-34</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-18.41797052920601</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7.427065307429028e-34</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-18.47688141630214</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.746979485803795e-94</v>
+      </c>
+      <c r="I14" t="n">
+        <v>-20.62186361206629</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
@@ -720,12 +876,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>6.033763570825231e-19</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-11.03823016902649</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4.877619006262921e-19</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-11.08088976195152</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3.428716862694029e-46</v>
+      </c>
+      <c r="I15" t="n">
+        <v>-14.26870808063906</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
@@ -735,12 +903,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="D16" t="n">
+        <v>1.383294227786068e-12</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-8.111621148101893</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.250665561943786e-12</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-8.132005276030474</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4.446755680268373e-22</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-9.660273413130227</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -758,12 +938,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>0.7250944363570428</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.3526581547446151</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.7298586230666879</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-0.3462913991185775</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.1694330516517278</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-1.374027801282287</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
@@ -773,12 +965,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>6.60178979776149e-13</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-8.261022671281603</v>
+      </c>
+      <c r="F18" t="n">
+        <v>7.2371352093527e-13</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-8.24248863306963</v>
+      </c>
+      <c r="H18" t="n">
+        <v>9.699379503933094e-47</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-14.35650713081258</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
@@ -788,12 +992,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>2.450786905087592e-12</v>
+      </c>
+      <c r="E19" t="n">
+        <v>7.995778985576518</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2.332301117228565e-12</v>
+      </c>
+      <c r="G19" t="n">
+        <v>8.005827734243461</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2.267058630030397e-23</v>
+      </c>
+      <c r="I19" t="n">
+        <v>9.960593237772516</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
@@ -803,12 +1019,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>1.198820482832236e-19</v>
+      </c>
+      <c r="E20" t="n">
+        <v>11.3628545532098</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.060371384519449e-19</v>
+      </c>
+      <c r="G20" t="n">
+        <v>11.38755889358876</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3.600043122826306e-98</v>
+      </c>
+      <c r="I20" t="n">
+        <v>21.02847951989557</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
@@ -818,12 +1046,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>2.89045986434642e-26</v>
+      </c>
+      <c r="E21" t="n">
+        <v>14.51849836528713</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2.749088100169913e-26</v>
+      </c>
+      <c r="G21" t="n">
+        <v>14.52925825514768</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2.45051128833605e-152</v>
+      </c>
+      <c r="I21" t="n">
+        <v>26.29068997363049</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
@@ -837,12 +1077,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>0.449700886261551</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.7589244724912581</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.4506161356762867</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.7573884104067238</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.3020816294876247</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1.031979695441616</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
@@ -852,12 +1104,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>1.083787437413268e-22</v>
+      </c>
+      <c r="E23" t="n">
+        <v>12.78925718769875</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.015152247192677e-22</v>
+      </c>
+      <c r="G23" t="n">
+        <v>12.80274624848467</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.145747613211451e-85</v>
+      </c>
+      <c r="I23" t="n">
+        <v>19.61524889266831</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
@@ -867,12 +1131,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>1.594510999367085e-24</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-13.6671664016932</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.127809253014935e-24</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-13.7399935807756</v>
+      </c>
+      <c r="H24" t="n">
+        <v>3.448874537135098e-64</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-16.91566738916881</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
@@ -882,12 +1158,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>3.508730133619444e-17</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-10.22647853355569</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3.415453042052321e-17</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-10.23184714951807</v>
+      </c>
+      <c r="H25" t="n">
+        <v>8.078396812895914e-37</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-12.67555586889975</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
@@ -897,12 +1185,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>3.459001370453729e-13</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-8.391221469003233</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3.232559184079042e-13</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-8.404842451397483</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.967697537551868e-24</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-10.20073889177335</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
@@ -916,12 +1216,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
+      <c r="D27" t="n">
+        <v>0.09806273438610065</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.670078695653618</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.09777564184879486</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1.671527508024842</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.001797748987947485</v>
+      </c>
+      <c r="I27" t="n">
+        <v>3.121757590647723</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
@@ -931,12 +1243,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>3.312212434473853e-25</v>
+      </c>
+      <c r="E28" t="n">
+        <v>13.99868179976036</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3.21509844933544e-25</v>
+      </c>
+      <c r="G28" t="n">
+        <v>14.00498471649352</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.164400600237484e-82</v>
+      </c>
+      <c r="I28" t="n">
+        <v>19.25997263570464</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
@@ -946,12 +1270,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>4.332501697042375e-26</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-14.43176323562077</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3.285442175192015e-26</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-14.49102844204121</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.08385542624827e-55</v>
+      </c>
+      <c r="I29" t="n">
+        <v>-15.72112292988057</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
@@ -961,12 +1297,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>2.748355541287907e-12</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-7.972532095144198</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2.560329816549957e-12</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-7.986909875329673</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2.224369570431324e-19</v>
+      </c>
+      <c r="I30" t="n">
+        <v>-9.001607288118187</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
@@ -976,12 +1324,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>1.203705981080514e-09</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-6.713620184247353</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1.045200785586313e-09</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-6.743577392133659</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.142829168509119e-13</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-7.423247515698832</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -999,12 +1359,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
+      <c r="D32" t="n">
+        <v>0.6513243923093057</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.4533004802847371</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.6023239518473503</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.5227387883206689</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.66542483236262e-09</v>
+      </c>
+      <c r="I32" t="n">
+        <v>-6.027473561844255</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
@@ -1014,12 +1386,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
+      <c r="D33" t="n">
+        <v>4.426993422742509e-05</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-4.273736144967675</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.716893839274386e-05</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-4.256959675134015</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1.944160912744482e-48</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-14.6250541681339</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
@@ -1029,12 +1413,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>5.921983662915415e-10</v>
+      </c>
+      <c r="E34" t="n">
+        <v>6.863677438333236</v>
+      </c>
+      <c r="F34" t="n">
+        <v>5.366641695727211e-10</v>
+      </c>
+      <c r="G34" t="n">
+        <v>6.884424848094099</v>
+      </c>
+      <c r="H34" t="n">
+        <v>3.619842062095687e-13</v>
+      </c>
+      <c r="I34" t="n">
+        <v>7.269064998970753</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
@@ -1044,12 +1440,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>9.931007518865216e-09</v>
+      </c>
+      <c r="E35" t="n">
+        <v>6.26007452013264</v>
+      </c>
+      <c r="F35" t="n">
+        <v>6.878644209461455e-09</v>
+      </c>
+      <c r="G35" t="n">
+        <v>6.339851911238164</v>
+      </c>
+      <c r="H35" t="n">
+        <v>8.776213819327987e-06</v>
+      </c>
+      <c r="I35" t="n">
+        <v>4.445317544515205</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
@@ -1059,12 +1467,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>3.152485915165974e-11</v>
+      </c>
+      <c r="E36" t="n">
+        <v>7.474154883476738</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1.946512588870831e-11</v>
+      </c>
+      <c r="G36" t="n">
+        <v>7.57322018166273</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1.359744610014487e-20</v>
+      </c>
+      <c r="I36" t="n">
+        <v>9.303439372870033</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
@@ -1078,12 +1498,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>0.8206610822257139</v>
+      </c>
+      <c r="E37" t="n">
+        <v>-0.2272975815729635</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.8071420686661308</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-0.2447688034595139</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.01853955266289848</v>
+      </c>
+      <c r="I37" t="n">
+        <v>2.354662158573957</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
@@ -1093,12 +1525,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>2.545706600489061e-16</v>
+      </c>
+      <c r="E38" t="n">
+        <v>9.831873189494425</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2.644981784824378e-16</v>
+      </c>
+      <c r="G38" t="n">
+        <v>9.824258693517145</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.064957364806026e-76</v>
+      </c>
+      <c r="I38" t="n">
+        <v>18.5356497230924</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
@@ -1108,12 +1552,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>4.98564227554142e-20</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-11.53965358965215</v>
+      </c>
+      <c r="F39" t="n">
+        <v>4.037916340498724e-20</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-11.58220308401793</v>
+      </c>
+      <c r="H39" t="n">
+        <v>6.385802609249861e-41</v>
+      </c>
+      <c r="I39" t="n">
+        <v>-13.3959450032712</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n"/>
@@ -1123,12 +1579,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
+      <c r="D40" t="n">
+        <v>1.883696732461173e-13</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-8.51337849731228</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1.360504651791749e-13</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-8.578685549038562</v>
+      </c>
+      <c r="H40" t="n">
+        <v>3.55483481813376e-33</v>
+      </c>
+      <c r="I40" t="n">
+        <v>-11.99995643591017</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
@@ -1138,12 +1606,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>3.380163938364885e-11</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-7.459800887283832</v>
+      </c>
+      <c r="F41" t="n">
+        <v>2.507467647484149e-11</v>
+      </c>
+      <c r="G41" t="n">
+        <v>-7.521228615912089</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2.779840564185298e-24</v>
+      </c>
+      <c r="I41" t="n">
+        <v>-10.16712811845961</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
@@ -1157,12 +1637,24 @@
           <t>[-20, 20]</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>0.4134070361069752</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.8213737475870581</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.4238891258992578</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.8030161034643183</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.001202863489806678</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3.238200247049615</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
@@ -1172,12 +1664,24 @@
           <t>[-20, -1]</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>3.266745023936181e-19</v>
+      </c>
+      <c r="E43" t="n">
+        <v>11.16133776943807</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3.150642179847639e-19</v>
+      </c>
+      <c r="G43" t="n">
+        <v>11.16860383310513</v>
+      </c>
+      <c r="H43" t="n">
+        <v>3.136012987472142e-72</v>
+      </c>
+      <c r="I43" t="n">
+        <v>17.97361434964883</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
@@ -1187,12 +1691,24 @@
           <t>[0, 20]</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
+      <c r="D44" t="n">
+        <v>8.318143406224688e-21</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-11.90189995577377</v>
+      </c>
+      <c r="F44" t="n">
+        <v>6.895126455633384e-21</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-11.93997231038679</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1.36078074810546e-48</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-14.64931630676763</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
@@ -1202,12 +1718,24 @@
           <t>[0, 5]</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>2.103434736550075e-11</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-7.557311030255744</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1.815868017889601e-11</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-7.587469526599441</v>
+      </c>
+      <c r="H45" t="n">
+        <v>3.102525580461644e-25</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-10.37861212530946</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
@@ -1217,12 +1745,24 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>5.64618343449275e-06</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-4.799148520658988</v>
+      </c>
+      <c r="F46" t="n">
+        <v>5.173119495764484e-06</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-4.820740771821624</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2.140741304251899e-13</v>
+      </c>
+      <c r="I46" t="n">
+        <v>-7.339699385852787</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>